<commit_message>
register / user Controller modify
</commit_message>
<xml_diff>
--- a/source/register_example.xlsx
+++ b/source/register_example.xlsx
@@ -9,12 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11840" yWindow="840" windowWidth="13720" windowHeight="13040" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="11840" yWindow="840" windowWidth="13720" windowHeight="13040" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mentor" sheetId="3" r:id="rId1"/>
     <sheet name="Mentee" sheetId="1" r:id="rId2"/>
-    <sheet name="Project_1-1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>SW Maestro</t>
   </si>
@@ -61,67 +60,25 @@
     <t>웹</t>
   </si>
   <si>
-    <t>mentor0@gmail.com</t>
-  </si>
-  <si>
     <t>어딘가</t>
   </si>
   <si>
     <t>010-000-0000</t>
   </si>
   <si>
-    <t>단계</t>
-  </si>
-  <si>
-    <t>차수</t>
-  </si>
-  <si>
-    <t>Mentor</t>
-  </si>
-  <si>
-    <t>Project Title</t>
-  </si>
-  <si>
-    <t>Field</t>
-  </si>
-  <si>
-    <t>Mentee</t>
-  </si>
-  <si>
-    <t>mentee00@gmail.com</t>
-  </si>
-  <si>
-    <t>web</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>이멘티</t>
-  </si>
-  <si>
-    <t>민멘티</t>
-  </si>
-  <si>
-    <t>강멘티</t>
-  </si>
-  <si>
-    <t>김멘토</t>
-  </si>
-  <si>
-    <t>김멘토의프로젝트 1단계 1차</t>
-  </si>
-  <si>
     <t>Somewhere</t>
   </si>
   <si>
-    <t>MENTEE_TEST</t>
-  </si>
-  <si>
-    <t>MENTOR_TEST</t>
-  </si>
-  <si>
-    <t>PROJECT_TEST</t>
+    <t>육멘토</t>
+  </si>
+  <si>
+    <t>mentor666@gmail.com</t>
+  </si>
+  <si>
+    <t>육멘티</t>
+  </si>
+  <si>
+    <t>mentee66@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -208,22 +165,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Style 1" xfId="1"/>
   </cellStyles>
@@ -510,7 +470,7 @@
   <dimension ref="A2:E8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -565,16 +525,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -590,8 +550,8 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A2:D8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -642,112 +602,23 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
-        <v>28</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A2:H9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:8" ht="37" x14ac:dyDescent="0.45">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>